<commit_message>
[REF] Tools refactoring: z0lib
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice.xlsx
+++ b/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="92">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -94,24 +94,30 @@
     <t xml:space="preserve">z0bug.invoice_PY_2</t>
   </si>
   <si>
+    <t xml:space="preserve">z0bug.res_partner_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contratto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.invoice_Z0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1/2021/0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">####-&lt;#-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.bank_company_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.invoice_Z0_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.res_partner_2</t>
   </si>
   <si>
-    <t xml:space="preserve">z0bug.invoice_Z0_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1/2021/0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">####-&lt;#-99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.bank_company_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.invoice_Z0_2</t>
-  </si>
-  <si>
     <t xml:space="preserve">SO123</t>
   </si>
   <si>
@@ -224,9 +230,6 @@
   </si>
   <si>
     <t xml:space="preserve">z0bug.invoice_ZI_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z0bug.res_partner_3</t>
   </si>
   <si>
     <t xml:space="preserve">XE125432</t>
@@ -419,7 +422,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,10 +534,10 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
@@ -563,20 +566,20 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -600,25 +603,25 @@
         <v>22</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>18</v>
@@ -642,25 +645,25 @@
         <v>22</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -678,31 +681,31 @@
         <v>20</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>18</v>
@@ -720,21 +723,21 @@
         <v>20</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
@@ -744,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>18</v>
@@ -770,20 +773,20 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>18</v>
@@ -801,7 +804,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>22</v>
@@ -809,20 +812,20 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>18</v>
@@ -834,7 +837,7 @@
         <v>18</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>20</v>
@@ -848,20 +851,20 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>18</v>
@@ -885,40 +888,40 @@
         <v>22</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>21</v>
@@ -929,35 +932,35 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>21</v>
@@ -968,35 +971,35 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>21</v>
@@ -1007,23 +1010,23 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>18</v>
@@ -1032,10 +1035,10 @@
         <v>18</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>21</v>
@@ -1046,23 +1049,23 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>18</v>
@@ -1071,10 +1074,10 @@
         <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>21</v>
@@ -1085,23 +1088,23 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>18</v>
@@ -1110,10 +1113,10 @@
         <v>18</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>21</v>
@@ -1124,23 +1127,23 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>18</v>
@@ -1149,13 +1152,13 @@
         <v>18</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>22</v>
@@ -1163,23 +1166,23 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>18</v>
@@ -1188,10 +1191,10 @@
         <v>18</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>21</v>
@@ -1202,38 +1205,38 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[IMP] install with odoo-module-migrate
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice.xlsx
+++ b/z0bug_odoo/build/lib/z0bug_odoo/data/account_invoice.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="114">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t xml:space="preserve">TI-8778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">####-&lt;#-27</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.fiscalpos_xx</t>
@@ -529,11 +532,11 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="S21" activeCellId="0" sqref="S21"/>
+      <selection pane="bottomRight" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1485,7 +1488,7 @@
         <v>107</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>38</v>
@@ -1503,7 +1506,7 @@
         <v>77</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>27</v>
@@ -1517,20 +1520,20 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>38</v>
@@ -1539,7 +1542,7 @@
         <v>23</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>76</v>

</xml_diff>